<commit_message>
WIP on #487 and other cleanup of tests.
</commit_message>
<xml_diff>
--- a/tests/assets/commented_csvs_test/test_excel_file_commented_row.xlsx
+++ b/tests/assets/commented_csvs_test/test_excel_file_commented_row.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">First description</t>
   </si>
   <si>
-    <t xml:space="preserve">25</t>
+    <t xml:space="preserve">Image</t>
   </si>
   <si>
     <t xml:space="preserve">0002</t>
@@ -55,9 +55,6 @@
     <t xml:space="preserve">Second description</t>
   </si>
   <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
     <t xml:space="preserve">#0003</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t xml:space="preserve">Third description</t>
   </si>
   <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
     <t xml:space="preserve">0004</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
   </si>
   <si>
     <t xml:space="preserve">Fourth description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28</t>
   </si>
   <si>
     <t xml:space="preserve">#0005</t>
@@ -191,33 +182,31 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,70 +248,70 @@
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>